<commit_message>
added arctic control units, points and meteostations
</commit_message>
<xml_diff>
--- a/satinfo.xlsx
+++ b/satinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\start\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\repos\sat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B969E7-9863-4B86-804F-0C4354CF1A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A4F777-79B6-43B3-872E-DF89C4C2179F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="2028" windowWidth="17232" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -1017,7 +1017,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1235,15 +1235,17 @@
   </sheetPr>
   <dimension ref="A1:O1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="7" width="14.44140625" customWidth="1"/>
+    <col min="4" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>